<commit_message>
nouveau Print de l'environnement et amélioration simple_exec
</commit_message>
<xml_diff>
--- a/resultats/simple_execution.xlsx
+++ b/resultats/simple_execution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\5A\OVR_SMA\TP2_tri_collectif_sma\SMA_TP2_Tri_Collectif\resultats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A062D6C6-273C-4638-AAC3-00ED0A7C0108}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10892657-24DA-4571-9A2A-8E537B53537D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{6B8A2C51-0B39-47A0-BD50-7946639C6253}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6B8A2C51-0B39-47A0-BD50-7946639C6253}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>exnombre moyen d'objets similiaires proches selon le nombre d'agents et le nombre d'itérations</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>taille grille</t>
   </si>
@@ -56,7 +53,13 @@
     <t>nb moyen de voisins similaire</t>
   </si>
   <si>
-    <t>ration objet isolé</t>
+    <t>nombre moyen d'objets similiaires proches selon le nombre d'agents et le nombre d'itérations</t>
+  </si>
+  <si>
+    <t>20*60</t>
+  </si>
+  <si>
+    <t>ratio objet isolé</t>
   </si>
 </sst>
 </file>
@@ -127,6 +130,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>nb moyen de voisins similaire selon l'itération</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -198,304 +226,304 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110</c:v>
+                  <c:v>11000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120</c:v>
+                  <c:v>12000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>130</c:v>
+                  <c:v>13000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>140</c:v>
+                  <c:v>14000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>150</c:v>
+                  <c:v>15000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>160</c:v>
+                  <c:v>16000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>170</c:v>
+                  <c:v>17000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>180</c:v>
+                  <c:v>18000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>190</c:v>
+                  <c:v>19000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>200</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>210</c:v>
+                  <c:v>21000</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>220</c:v>
+                  <c:v>22000</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>230</c:v>
+                  <c:v>23000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>240</c:v>
+                  <c:v>24000</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>250</c:v>
+                  <c:v>25000</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>260</c:v>
+                  <c:v>26000</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>270</c:v>
+                  <c:v>27000</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>280</c:v>
+                  <c:v>28000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>290</c:v>
+                  <c:v>29000</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>300</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>310</c:v>
+                  <c:v>31000</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>320</c:v>
+                  <c:v>32000</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>330</c:v>
+                  <c:v>33000</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>340</c:v>
+                  <c:v>34000</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>350</c:v>
+                  <c:v>35000</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>360</c:v>
+                  <c:v>36000</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>370</c:v>
+                  <c:v>37000</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>380</c:v>
+                  <c:v>38000</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>390</c:v>
+                  <c:v>39000</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>400</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>410</c:v>
+                  <c:v>41000</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>420</c:v>
+                  <c:v>42000</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>430</c:v>
+                  <c:v>43000</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>440</c:v>
+                  <c:v>44000</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>450</c:v>
+                  <c:v>45000</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>460</c:v>
+                  <c:v>46000</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>470</c:v>
+                  <c:v>47000</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>480</c:v>
+                  <c:v>48000</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>490</c:v>
+                  <c:v>49000</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>500</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>510</c:v>
+                  <c:v>51000</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>520</c:v>
+                  <c:v>52000</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>530</c:v>
+                  <c:v>53000</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>540</c:v>
+                  <c:v>54000</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>550</c:v>
+                  <c:v>55000</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>560</c:v>
+                  <c:v>56000</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>570</c:v>
+                  <c:v>57000</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>580</c:v>
+                  <c:v>58000</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>590</c:v>
+                  <c:v>59000</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>600</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>610</c:v>
+                  <c:v>61000</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>620</c:v>
+                  <c:v>62000</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>630</c:v>
+                  <c:v>63000</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>640</c:v>
+                  <c:v>64000</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>650</c:v>
+                  <c:v>65000</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>660</c:v>
+                  <c:v>66000</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>670</c:v>
+                  <c:v>67000</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>680</c:v>
+                  <c:v>68000</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>690</c:v>
+                  <c:v>69000</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>700</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>710</c:v>
+                  <c:v>71000</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>720</c:v>
+                  <c:v>72000</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>730</c:v>
+                  <c:v>73000</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>740</c:v>
+                  <c:v>74000</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>750</c:v>
+                  <c:v>75000</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>760</c:v>
+                  <c:v>76000</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>770</c:v>
+                  <c:v>77000</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>780</c:v>
+                  <c:v>78000</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>790</c:v>
+                  <c:v>79000</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>800</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>810</c:v>
+                  <c:v>81000</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>820</c:v>
+                  <c:v>82000</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>830</c:v>
+                  <c:v>83000</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>840</c:v>
+                  <c:v>84000</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>850</c:v>
+                  <c:v>85000</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>860</c:v>
+                  <c:v>86000</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>870</c:v>
+                  <c:v>87000</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>880</c:v>
+                  <c:v>88000</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>890</c:v>
+                  <c:v>89000</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>900</c:v>
+                  <c:v>90000</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>910</c:v>
+                  <c:v>91000</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>920</c:v>
+                  <c:v>92000</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>930</c:v>
+                  <c:v>93000</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>940</c:v>
+                  <c:v>94000</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>950</c:v>
+                  <c:v>95000</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>960</c:v>
+                  <c:v>96000</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>970</c:v>
+                  <c:v>97000</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>980</c:v>
+                  <c:v>98000</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>990</c:v>
+                  <c:v>99000</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -507,307 +535,307 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>1.02857142857142</c:v>
+                  <c:v>1.04729729729729</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1142857142857101</c:v>
+                  <c:v>1.93150684931506</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.09374999999999</c:v>
+                  <c:v>2.0212014134275602</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.24242424242424</c:v>
+                  <c:v>2.2291666666666599</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2615384615384599</c:v>
+                  <c:v>2.3505154639175201</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3333333333333299</c:v>
+                  <c:v>2.45205479452054</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3548387096774199</c:v>
+                  <c:v>2.2749140893470701</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.32258064516129</c:v>
+                  <c:v>2.4041095890410902</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3548387096774099</c:v>
+                  <c:v>2.38356164383561</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.28813559322033</c:v>
+                  <c:v>2.52027027027026</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.34426229508196</c:v>
+                  <c:v>2.4166666666666599</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.5757575757575699</c:v>
+                  <c:v>2.5951557093425599</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.53125</c:v>
+                  <c:v>2.38907849829351</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.59375</c:v>
+                  <c:v>2.5753424657534199</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.6307692307692301</c:v>
+                  <c:v>2.4513888888888902</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.5454545454545401</c:v>
+                  <c:v>2.39175257731958</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.65625</c:v>
+                  <c:v>2.5586206896551702</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6610169491525399</c:v>
+                  <c:v>2.3611111111111098</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.6451612903225801</c:v>
+                  <c:v>2.4844290657439401</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.76119402985074</c:v>
+                  <c:v>2.55555555555555</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.6825396825396799</c:v>
+                  <c:v>2.5034965034965002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.63333333333333</c:v>
+                  <c:v>2.69655172413793</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.7538461538461501</c:v>
+                  <c:v>2.6968641114982499</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.7538461538461501</c:v>
+                  <c:v>2.7735191637630598</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.7777777777777699</c:v>
+                  <c:v>2.51748251748251</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.7096774193548301</c:v>
+                  <c:v>2.5517241379310298</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.7846153846153801</c:v>
+                  <c:v>2.5314685314685299</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.71428571428571</c:v>
+                  <c:v>2.50859106529209</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.84375</c:v>
+                  <c:v>2.7379310344827501</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.80645161290322</c:v>
+                  <c:v>2.7944250871080101</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.87096774193548</c:v>
+                  <c:v>2.7216494845360799</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.8387096774193501</c:v>
+                  <c:v>2.7010309278350499</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.9375</c:v>
+                  <c:v>2.5103448275861999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.99999999999999</c:v>
+                  <c:v>2.5347222222222201</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2</c:v>
+                  <c:v>2.7404844290657402</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.0624999999999898</c:v>
+                  <c:v>2.5972222222222201</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.0317460317460299</c:v>
+                  <c:v>2.5517241379310298</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.99999999999999</c:v>
+                  <c:v>2.54794520547944</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.0923076923076902</c:v>
+                  <c:v>2.5296167247386698</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.9365079365079301</c:v>
+                  <c:v>2.6574394463667801</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.84374999999999</c:v>
+                  <c:v>2.5486111111111098</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.87692307692307</c:v>
+                  <c:v>2.6713286713286699</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.9076923076923</c:v>
+                  <c:v>2.6643356643356602</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.9032258064516101</c:v>
+                  <c:v>2.5724137931034399</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.96923076923076</c:v>
+                  <c:v>2.63448275862069</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.9365079365079301</c:v>
+                  <c:v>2.6275862068965501</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.9365079365079301</c:v>
+                  <c:v>2.7191780821917799</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.8305084745762701</c:v>
+                  <c:v>2.66896551724138</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.86666666666666</c:v>
+                  <c:v>2.5782312925170001</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.87096774193548</c:v>
+                  <c:v>2.6827586206896501</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.87692307692307</c:v>
+                  <c:v>2.6643598615916901</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.8125</c:v>
+                  <c:v>2.6484641638225201</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.9047619047619</c:v>
+                  <c:v>2.6666666666666599</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.96969696969696</c:v>
+                  <c:v>2.7291666666666599</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.96923076923076</c:v>
+                  <c:v>2.8373702422145302</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.8412698412698401</c:v>
+                  <c:v>2.66891891891891</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.84848484848484</c:v>
+                  <c:v>2.6482758620689602</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.0579710144927499</c:v>
+                  <c:v>2.7859649122807002</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.0579710144927499</c:v>
+                  <c:v>2.7298245614034999</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.0298507462686501</c:v>
+                  <c:v>2.63448275862069</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2.0289855072463698</c:v>
+                  <c:v>2.8503401360544198</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1.9393939393939399</c:v>
+                  <c:v>2.8191126279863399</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2.0307692307692302</c:v>
+                  <c:v>2.8333333333333299</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2.0895522388059602</c:v>
+                  <c:v>2.8356164383561602</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.9375</c:v>
+                  <c:v>2.7386759581881499</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.94029850746268</c:v>
+                  <c:v>2.8432055749128899</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.84848484848484</c:v>
+                  <c:v>2.9652777777777701</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.8208955223880501</c:v>
+                  <c:v>2.9379310344827498</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1.7878787878787801</c:v>
+                  <c:v>2.8464163822525599</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1.7538461538461501</c:v>
+                  <c:v>2.8741258741258702</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1.65625</c:v>
+                  <c:v>2.8512110726643498</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.7538461538461501</c:v>
+                  <c:v>3.0206896551724101</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1.6969696969696899</c:v>
+                  <c:v>2.8996539792387499</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1.8805970149253699</c:v>
+                  <c:v>2.8934707903780001</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1.9090909090909001</c:v>
+                  <c:v>2.9762711864406701</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1.97058823529411</c:v>
+                  <c:v>2.86219081272084</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1.99999999999999</c:v>
+                  <c:v>2.9484536082474202</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>2.0857142857142801</c:v>
+                  <c:v>2.9140893470790301</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>2.02941176470588</c:v>
+                  <c:v>2.8827586206896498</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>2</c:v>
+                  <c:v>3.0779661016949098</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.94029850746268</c:v>
+                  <c:v>2.90592334494773</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>2.0588235294117601</c:v>
+                  <c:v>2.95138888888888</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2.0303030303030298</c:v>
+                  <c:v>2.91525423728813</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>2</c:v>
+                  <c:v>2.9895470383275198</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>2.12307692307692</c:v>
+                  <c:v>3.0209790209790199</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>2.09523809523809</c:v>
+                  <c:v>2.8689655172413802</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>2.1538461538461502</c:v>
+                  <c:v>2.8532423208191098</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>2.24615384615384</c:v>
+                  <c:v>2.9010238907849799</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2.2903225806451601</c:v>
+                  <c:v>3.1095890410958802</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>2.2769230769230702</c:v>
+                  <c:v>3.0726643598615899</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2.29850746268656</c:v>
+                  <c:v>2.9863013698630101</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>2.2089552238805901</c:v>
+                  <c:v>2.9965397923875399</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>2.1714285714285699</c:v>
+                  <c:v>3.0174216027874499</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>2.0303030303030298</c:v>
+                  <c:v>2.8482758620689599</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.9076923076923</c:v>
+                  <c:v>2.8041237113402002</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.99999999999999</c:v>
+                  <c:v>2.8384879725085899</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1.96923076923076</c:v>
+                  <c:v>2.8767123287671201</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2.15151515151515</c:v>
+                  <c:v>2.8591065292096198</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.99999999999999</c:v>
+                  <c:v>2.9241379310344802</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2.14925373134328</c:v>
+                  <c:v>3.0311418685120999</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>2.0923076923076902</c:v>
+                  <c:v>2.9862068965517201</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -838,6 +866,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>itération</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -903,6 +986,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>nb moyen de voisins similaire</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -998,6 +1136,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ratio objet isolé selon</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> l'itération</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1042,7 +1210,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ration objet isolé</c:v>
+                  <c:v>ratio objet isolé</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1069,304 +1237,304 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110</c:v>
+                  <c:v>11000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120</c:v>
+                  <c:v>12000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>130</c:v>
+                  <c:v>13000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>140</c:v>
+                  <c:v>14000</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>150</c:v>
+                  <c:v>15000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>160</c:v>
+                  <c:v>16000</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>170</c:v>
+                  <c:v>17000</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>180</c:v>
+                  <c:v>18000</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>190</c:v>
+                  <c:v>19000</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>200</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>210</c:v>
+                  <c:v>21000</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>220</c:v>
+                  <c:v>22000</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>230</c:v>
+                  <c:v>23000</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>240</c:v>
+                  <c:v>24000</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>250</c:v>
+                  <c:v>25000</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>260</c:v>
+                  <c:v>26000</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>270</c:v>
+                  <c:v>27000</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>280</c:v>
+                  <c:v>28000</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>290</c:v>
+                  <c:v>29000</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>300</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>310</c:v>
+                  <c:v>31000</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>320</c:v>
+                  <c:v>32000</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>330</c:v>
+                  <c:v>33000</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>340</c:v>
+                  <c:v>34000</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>350</c:v>
+                  <c:v>35000</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>360</c:v>
+                  <c:v>36000</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>370</c:v>
+                  <c:v>37000</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>380</c:v>
+                  <c:v>38000</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>390</c:v>
+                  <c:v>39000</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>400</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>410</c:v>
+                  <c:v>41000</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>420</c:v>
+                  <c:v>42000</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>430</c:v>
+                  <c:v>43000</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>440</c:v>
+                  <c:v>44000</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>450</c:v>
+                  <c:v>45000</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>460</c:v>
+                  <c:v>46000</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>470</c:v>
+                  <c:v>47000</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>480</c:v>
+                  <c:v>48000</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>490</c:v>
+                  <c:v>49000</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>500</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>510</c:v>
+                  <c:v>51000</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>520</c:v>
+                  <c:v>52000</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>530</c:v>
+                  <c:v>53000</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>540</c:v>
+                  <c:v>54000</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>550</c:v>
+                  <c:v>55000</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>560</c:v>
+                  <c:v>56000</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>570</c:v>
+                  <c:v>57000</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>580</c:v>
+                  <c:v>58000</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>590</c:v>
+                  <c:v>59000</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>600</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>610</c:v>
+                  <c:v>61000</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>620</c:v>
+                  <c:v>62000</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>630</c:v>
+                  <c:v>63000</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>640</c:v>
+                  <c:v>64000</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>650</c:v>
+                  <c:v>65000</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>660</c:v>
+                  <c:v>66000</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>670</c:v>
+                  <c:v>67000</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>680</c:v>
+                  <c:v>68000</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>690</c:v>
+                  <c:v>69000</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>700</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>710</c:v>
+                  <c:v>71000</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>720</c:v>
+                  <c:v>72000</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>730</c:v>
+                  <c:v>73000</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>740</c:v>
+                  <c:v>74000</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>750</c:v>
+                  <c:v>75000</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>760</c:v>
+                  <c:v>76000</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>770</c:v>
+                  <c:v>77000</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>780</c:v>
+                  <c:v>78000</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>790</c:v>
+                  <c:v>79000</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>800</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>810</c:v>
+                  <c:v>81000</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>820</c:v>
+                  <c:v>82000</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>830</c:v>
+                  <c:v>83000</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>840</c:v>
+                  <c:v>84000</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>850</c:v>
+                  <c:v>85000</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>860</c:v>
+                  <c:v>86000</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>870</c:v>
+                  <c:v>87000</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>880</c:v>
+                  <c:v>88000</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>890</c:v>
+                  <c:v>89000</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>900</c:v>
+                  <c:v>90000</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>910</c:v>
+                  <c:v>91000</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>920</c:v>
+                  <c:v>92000</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>930</c:v>
+                  <c:v>93000</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>940</c:v>
+                  <c:v>94000</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>950</c:v>
+                  <c:v>95000</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>960</c:v>
+                  <c:v>96000</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>970</c:v>
+                  <c:v>97000</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>980</c:v>
+                  <c:v>98000</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>990</c:v>
+                  <c:v>99000</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1378,307 +1546,307 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>0.24285714285714199</c:v>
+                  <c:v>0.28378378378378299</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>5.8219178082191701E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.203125</c:v>
+                  <c:v>4.2402826855123602E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13636363636363599</c:v>
+                  <c:v>2.43055555555555E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15384615384615299</c:v>
+                  <c:v>2.40549828178694E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13636363636363599</c:v>
+                  <c:v>2.0547945205479399E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12903225806451599</c:v>
+                  <c:v>2.06185567010309E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.14516129032257999</c:v>
+                  <c:v>3.7671232876712299E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.112903225806451</c:v>
+                  <c:v>3.7671232876712299E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.169491525423728</c:v>
+                  <c:v>1.0135135135135099E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.16393442622950799</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.10606060606060599</c:v>
+                  <c:v>2.76816608996539E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.109375</c:v>
+                  <c:v>3.0716723549488002E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.109375</c:v>
+                  <c:v>6.8493150684931503E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.2307692307692299E-2</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.13636363636363599</c:v>
+                  <c:v>3.4364261168384799E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.8125E-2</c:v>
+                  <c:v>2.7586206896551699E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.4745762711864403E-2</c:v>
+                  <c:v>3.8194444444444399E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.8387096774193498E-2</c:v>
+                  <c:v>2.42214532871972E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.4925373134328301E-2</c:v>
+                  <c:v>1.04166666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.1746031746031703E-2</c:v>
+                  <c:v>2.44755244755244E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.05</c:v>
+                  <c:v>6.8965517241379301E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6.15384615384615E-2</c:v>
+                  <c:v>3.1358885017421602E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6.15384615384615E-2</c:v>
+                  <c:v>2.78745644599303E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.1746031746031703E-2</c:v>
+                  <c:v>3.1468531468531402E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.8387096774193498E-2</c:v>
+                  <c:v>1.0344827586206799E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.6153846153846101E-2</c:v>
+                  <c:v>2.09790209790209E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.3492063492063405E-2</c:v>
+                  <c:v>3.0927835051546299E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9.375E-2</c:v>
+                  <c:v>1.72413793103448E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.2258064516128997E-2</c:v>
+                  <c:v>1.39372822299651E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.8387096774193498E-2</c:v>
+                  <c:v>1.71821305841924E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.8387096774193498E-2</c:v>
+                  <c:v>2.40549828178694E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.6875E-2</c:v>
+                  <c:v>1.72413793103448E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.6875E-2</c:v>
+                  <c:v>2.43055555555555E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.0769230769230702E-2</c:v>
+                  <c:v>1.03806228373702E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.6875E-2</c:v>
+                  <c:v>2.0833333333333301E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6.3492063492063405E-2</c:v>
+                  <c:v>2.4137931034482699E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.6875E-2</c:v>
+                  <c:v>1.7123287671232799E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.6153846153846101E-2</c:v>
+                  <c:v>1.39372822299651E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.3492063492063405E-2</c:v>
+                  <c:v>1.03806228373702E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>7.8125E-2</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>6.15384615384615E-2</c:v>
+                  <c:v>1.3986013986013899E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>6.15384615384615E-2</c:v>
+                  <c:v>2.7972027972027899E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6.4516129032257993E-2</c:v>
+                  <c:v>3.1034482758620599E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4.6153846153846101E-2</c:v>
+                  <c:v>2.7586206896551699E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>6.3492063492063405E-2</c:v>
+                  <c:v>3.1034482758620599E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.7619047619047603E-2</c:v>
+                  <c:v>1.7123287671232799E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>8.4745762711864403E-2</c:v>
+                  <c:v>1.72413793103448E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.05</c:v>
+                  <c:v>2.7210884353741398E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.8387096774193498E-2</c:v>
+                  <c:v>3.4482758620689599E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>6.15384615384615E-2</c:v>
+                  <c:v>6.9204152249134898E-3</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>2.7303754266211601E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.7619047619047603E-2</c:v>
+                  <c:v>2.43055555555555E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.54545454545454E-2</c:v>
+                  <c:v>1.7361111111111101E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.107692307692307</c:v>
+                  <c:v>1.03806228373702E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>9.5238095238095205E-2</c:v>
+                  <c:v>1.35135135135135E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>6.0606060606060601E-2</c:v>
+                  <c:v>1.72413793103448E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>5.7971014492753603E-2</c:v>
+                  <c:v>1.7543859649122799E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4.3478260869565202E-2</c:v>
+                  <c:v>1.7543859649122799E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>4.4776119402985003E-2</c:v>
+                  <c:v>2.0689655172413699E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>5.7971014492753603E-2</c:v>
+                  <c:v>1.7006802721088399E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>6.0606060606060601E-2</c:v>
+                  <c:v>1.0238907849829299E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>6.15384615384615E-2</c:v>
+                  <c:v>2.43055555555555E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>5.9701492537313397E-2</c:v>
+                  <c:v>1.7123287671232799E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>3.125E-2</c:v>
+                  <c:v>1.74216027874564E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.4925373134328301E-2</c:v>
+                  <c:v>1.74216027874564E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.51515151515151E-2</c:v>
+                  <c:v>1.04166666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.4925373134328301E-2</c:v>
+                  <c:v>3.4482758620689599E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>4.54545454545454E-2</c:v>
+                  <c:v>1.7064846416382201E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>4.6153846153846101E-2</c:v>
+                  <c:v>1.04895104895104E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>2.42214532871972E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>6.15384615384615E-2</c:v>
+                  <c:v>6.8965517241379301E-3</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.10606060606060599</c:v>
+                  <c:v>1.03806228373702E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>2.9850746268656699E-2</c:v>
+                  <c:v>2.06185567010309E-2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1.51515151515151E-2</c:v>
+                  <c:v>1.01694915254237E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>5.8823529411764698E-2</c:v>
+                  <c:v>2.8268551236749099E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>4.4117647058823498E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>4.2857142857142802E-2</c:v>
+                  <c:v>2.06185567010309E-2</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>4.4117647058823498E-2</c:v>
+                  <c:v>1.3793103448275799E-2</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>2.9850746268656699E-2</c:v>
+                  <c:v>2.0338983050847401E-2</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>2.9850746268656699E-2</c:v>
+                  <c:v>1.0452961672473801E-2</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.47058823529411E-2</c:v>
+                  <c:v>3.4722222222222199E-3</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.51515151515151E-2</c:v>
+                  <c:v>1.01694915254237E-2</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>3.1746031746031703E-2</c:v>
+                  <c:v>1.39372822299651E-2</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>4.6153846153846101E-2</c:v>
+                  <c:v>3.49650349650349E-3</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>4.7619047619047603E-2</c:v>
+                  <c:v>6.8965517241379301E-3</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>6.15384615384615E-2</c:v>
+                  <c:v>1.36518771331058E-2</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>6.15384615384615E-2</c:v>
+                  <c:v>6.8259385665529002E-3</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>3.2258064516128997E-2</c:v>
+                  <c:v>1.7123287671232799E-2</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>3.0769230769230702E-2</c:v>
+                  <c:v>1.73010380622837E-2</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2.9850746268656699E-2</c:v>
+                  <c:v>6.8493150684931503E-3</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>2.9850746268656699E-2</c:v>
+                  <c:v>1.38408304498269E-2</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>4.2857142857142802E-2</c:v>
+                  <c:v>1.39372822299651E-2</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>6.0606060606060601E-2</c:v>
+                  <c:v>3.4482758620689598E-3</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>9.2307692307692299E-2</c:v>
+                  <c:v>6.8728522336769697E-3</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>5.9701492537313397E-2</c:v>
+                  <c:v>1.37457044673539E-2</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>6.15384615384615E-2</c:v>
+                  <c:v>1.0273972602739699E-2</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>4.54545454545454E-2</c:v>
+                  <c:v>1.37457044673539E-2</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>6.15384615384615E-2</c:v>
+                  <c:v>6.8965517241379301E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>4.4776119402985003E-2</c:v>
+                  <c:v>1.38408304498269E-2</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>3.0769230769230702E-2</c:v>
+                  <c:v>1.3793103448275799E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1709,6 +1877,64 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>itération</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1774,6 +2000,64 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>ratio objet isolé </a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2971,15 +3255,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3008,16 +3292,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3346,52 +3630,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8D0FC4-D921-4221-ADF4-2DC65EDAEE14}">
   <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>300</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="F2">
-        <v>36</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
       <c r="H2">
-        <v>24</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3399,1110 +3683,1110 @@
         <v>0</v>
       </c>
       <c r="B4" s="1">
-        <v>1.02857142857142</v>
+        <v>1.04729729729729</v>
       </c>
       <c r="C4" s="1">
-        <v>0.24285714285714199</v>
+        <v>0.28378378378378299</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="B5" s="1">
-        <v>1.1142857142857101</v>
+        <v>1.93150684931506</v>
       </c>
       <c r="C5" s="1">
-        <v>0.2</v>
+        <v>5.8219178082191701E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="B6" s="1">
-        <v>1.09374999999999</v>
+        <v>2.0212014134275602</v>
       </c>
       <c r="C6" s="1">
-        <v>0.203125</v>
+        <v>4.2402826855123602E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>30</v>
+        <v>3000</v>
       </c>
       <c r="B7" s="1">
-        <v>1.24242424242424</v>
+        <v>2.2291666666666599</v>
       </c>
       <c r="C7" s="1">
-        <v>0.13636363636363599</v>
+        <v>2.43055555555555E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>40</v>
+        <v>4000</v>
       </c>
       <c r="B8" s="1">
-        <v>1.2615384615384599</v>
+        <v>2.3505154639175201</v>
       </c>
       <c r="C8" s="1">
-        <v>0.15384615384615299</v>
+        <v>2.40549828178694E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>50</v>
+        <v>5000</v>
       </c>
       <c r="B9" s="1">
-        <v>1.3333333333333299</v>
+        <v>2.45205479452054</v>
       </c>
       <c r="C9" s="1">
-        <v>0.13636363636363599</v>
+        <v>2.0547945205479399E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>60</v>
+        <v>6000</v>
       </c>
       <c r="B10" s="1">
-        <v>1.3548387096774199</v>
+        <v>2.2749140893470701</v>
       </c>
       <c r="C10" s="1">
-        <v>0.12903225806451599</v>
+        <v>2.06185567010309E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>70</v>
+        <v>7000</v>
       </c>
       <c r="B11" s="1">
-        <v>1.32258064516129</v>
+        <v>2.4041095890410902</v>
       </c>
       <c r="C11" s="1">
-        <v>0.14516129032257999</v>
+        <v>3.7671232876712299E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>80</v>
+        <v>8000</v>
       </c>
       <c r="B12" s="1">
-        <v>1.3548387096774099</v>
+        <v>2.38356164383561</v>
       </c>
       <c r="C12" s="1">
-        <v>0.112903225806451</v>
+        <v>3.7671232876712299E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>90</v>
+        <v>9000</v>
       </c>
       <c r="B13" s="1">
-        <v>1.28813559322033</v>
+        <v>2.52027027027026</v>
       </c>
       <c r="C13" s="1">
-        <v>0.169491525423728</v>
+        <v>1.0135135135135099E-2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="B14" s="1">
-        <v>1.34426229508196</v>
+        <v>2.4166666666666599</v>
       </c>
       <c r="C14" s="1">
-        <v>0.16393442622950799</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>110</v>
+        <v>11000</v>
       </c>
       <c r="B15" s="1">
-        <v>1.5757575757575699</v>
+        <v>2.5951557093425599</v>
       </c>
       <c r="C15" s="1">
-        <v>0.10606060606060599</v>
+        <v>2.76816608996539E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>120</v>
+        <v>12000</v>
       </c>
       <c r="B16" s="1">
-        <v>1.53125</v>
+        <v>2.38907849829351</v>
       </c>
       <c r="C16" s="1">
-        <v>0.109375</v>
+        <v>3.0716723549488002E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>130</v>
+        <v>13000</v>
       </c>
       <c r="B17" s="1">
-        <v>1.59375</v>
+        <v>2.5753424657534199</v>
       </c>
       <c r="C17" s="1">
-        <v>0.109375</v>
+        <v>6.8493150684931503E-3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>140</v>
+        <v>14000</v>
       </c>
       <c r="B18" s="1">
-        <v>1.6307692307692301</v>
+        <v>2.4513888888888902</v>
       </c>
       <c r="C18" s="1">
-        <v>9.2307692307692299E-2</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>150</v>
+        <v>15000</v>
       </c>
       <c r="B19" s="1">
-        <v>1.5454545454545401</v>
+        <v>2.39175257731958</v>
       </c>
       <c r="C19" s="1">
-        <v>0.13636363636363599</v>
+        <v>3.4364261168384799E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>160</v>
+        <v>16000</v>
       </c>
       <c r="B20" s="1">
-        <v>1.65625</v>
+        <v>2.5586206896551702</v>
       </c>
       <c r="C20" s="1">
-        <v>7.8125E-2</v>
+        <v>2.7586206896551699E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>170</v>
+        <v>17000</v>
       </c>
       <c r="B21" s="1">
-        <v>1.6610169491525399</v>
+        <v>2.3611111111111098</v>
       </c>
       <c r="C21" s="1">
-        <v>8.4745762711864403E-2</v>
+        <v>3.8194444444444399E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>180</v>
+        <v>18000</v>
       </c>
       <c r="B22" s="1">
-        <v>1.6451612903225801</v>
+        <v>2.4844290657439401</v>
       </c>
       <c r="C22" s="1">
-        <v>4.8387096774193498E-2</v>
+        <v>2.42214532871972E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>190</v>
+        <v>19000</v>
       </c>
       <c r="B23" s="1">
-        <v>1.76119402985074</v>
+        <v>2.55555555555555</v>
       </c>
       <c r="C23" s="1">
-        <v>1.4925373134328301E-2</v>
+        <v>1.04166666666666E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>200</v>
+        <v>20000</v>
       </c>
       <c r="B24" s="1">
-        <v>1.6825396825396799</v>
+        <v>2.5034965034965002</v>
       </c>
       <c r="C24" s="1">
-        <v>3.1746031746031703E-2</v>
+        <v>2.44755244755244E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>210</v>
+        <v>21000</v>
       </c>
       <c r="B25" s="1">
-        <v>1.63333333333333</v>
+        <v>2.69655172413793</v>
       </c>
       <c r="C25" s="1">
-        <v>0.05</v>
+        <v>6.8965517241379301E-3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>220</v>
+        <v>22000</v>
       </c>
       <c r="B26" s="1">
-        <v>1.7538461538461501</v>
+        <v>2.6968641114982499</v>
       </c>
       <c r="C26" s="1">
-        <v>6.15384615384615E-2</v>
+        <v>3.1358885017421602E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>230</v>
+        <v>23000</v>
       </c>
       <c r="B27" s="1">
-        <v>1.7538461538461501</v>
+        <v>2.7735191637630598</v>
       </c>
       <c r="C27" s="1">
-        <v>6.15384615384615E-2</v>
+        <v>2.78745644599303E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>240</v>
+        <v>24000</v>
       </c>
       <c r="B28" s="1">
-        <v>1.7777777777777699</v>
+        <v>2.51748251748251</v>
       </c>
       <c r="C28" s="1">
-        <v>3.1746031746031703E-2</v>
+        <v>3.1468531468531402E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>250</v>
+        <v>25000</v>
       </c>
       <c r="B29" s="1">
-        <v>1.7096774193548301</v>
+        <v>2.5517241379310298</v>
       </c>
       <c r="C29" s="1">
-        <v>4.8387096774193498E-2</v>
+        <v>1.0344827586206799E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>260</v>
+        <v>26000</v>
       </c>
       <c r="B30" s="1">
-        <v>1.7846153846153801</v>
+        <v>2.5314685314685299</v>
       </c>
       <c r="C30" s="1">
-        <v>4.6153846153846101E-2</v>
+        <v>2.09790209790209E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>270</v>
+        <v>27000</v>
       </c>
       <c r="B31" s="1">
-        <v>1.71428571428571</v>
+        <v>2.50859106529209</v>
       </c>
       <c r="C31" s="1">
-        <v>6.3492063492063405E-2</v>
+        <v>3.0927835051546299E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>280</v>
+        <v>28000</v>
       </c>
       <c r="B32" s="1">
-        <v>1.84375</v>
+        <v>2.7379310344827501</v>
       </c>
       <c r="C32" s="1">
-        <v>9.375E-2</v>
+        <v>1.72413793103448E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>290</v>
+        <v>29000</v>
       </c>
       <c r="B33" s="1">
-        <v>1.80645161290322</v>
+        <v>2.7944250871080101</v>
       </c>
       <c r="C33" s="1">
-        <v>3.2258064516128997E-2</v>
+        <v>1.39372822299651E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>300</v>
+        <v>30000</v>
       </c>
       <c r="B34" s="1">
-        <v>1.87096774193548</v>
+        <v>2.7216494845360799</v>
       </c>
       <c r="C34" s="1">
-        <v>4.8387096774193498E-2</v>
+        <v>1.71821305841924E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>310</v>
+        <v>31000</v>
       </c>
       <c r="B35" s="1">
-        <v>1.8387096774193501</v>
+        <v>2.7010309278350499</v>
       </c>
       <c r="C35" s="1">
-        <v>4.8387096774193498E-2</v>
+        <v>2.40549828178694E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>320</v>
+        <v>32000</v>
       </c>
       <c r="B36" s="1">
-        <v>1.9375</v>
+        <v>2.5103448275861999</v>
       </c>
       <c r="C36" s="1">
-        <v>4.6875E-2</v>
+        <v>1.72413793103448E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>330</v>
+        <v>33000</v>
       </c>
       <c r="B37" s="1">
-        <v>1.99999999999999</v>
+        <v>2.5347222222222201</v>
       </c>
       <c r="C37" s="1">
-        <v>4.6875E-2</v>
+        <v>2.43055555555555E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>340</v>
+        <v>34000</v>
       </c>
       <c r="B38" s="1">
-        <v>2</v>
+        <v>2.7404844290657402</v>
       </c>
       <c r="C38" s="1">
-        <v>3.0769230769230702E-2</v>
+        <v>1.03806228373702E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>350</v>
+        <v>35000</v>
       </c>
       <c r="B39" s="1">
-        <v>2.0624999999999898</v>
+        <v>2.5972222222222201</v>
       </c>
       <c r="C39" s="1">
-        <v>4.6875E-2</v>
+        <v>2.0833333333333301E-2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>360</v>
+        <v>36000</v>
       </c>
       <c r="B40" s="1">
-        <v>2.0317460317460299</v>
+        <v>2.5517241379310298</v>
       </c>
       <c r="C40" s="1">
-        <v>6.3492063492063405E-2</v>
+        <v>2.4137931034482699E-2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>370</v>
+        <v>37000</v>
       </c>
       <c r="B41" s="1">
-        <v>1.99999999999999</v>
+        <v>2.54794520547944</v>
       </c>
       <c r="C41" s="1">
-        <v>4.6875E-2</v>
+        <v>1.7123287671232799E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>380</v>
+        <v>38000</v>
       </c>
       <c r="B42" s="1">
-        <v>2.0923076923076902</v>
+        <v>2.5296167247386698</v>
       </c>
       <c r="C42" s="1">
-        <v>4.6153846153846101E-2</v>
+        <v>1.39372822299651E-2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>390</v>
+        <v>39000</v>
       </c>
       <c r="B43" s="1">
-        <v>1.9365079365079301</v>
+        <v>2.6574394463667801</v>
       </c>
       <c r="C43" s="1">
-        <v>6.3492063492063405E-2</v>
+        <v>1.03806228373702E-2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>400</v>
+        <v>40000</v>
       </c>
       <c r="B44" s="1">
-        <v>1.84374999999999</v>
+        <v>2.5486111111111098</v>
       </c>
       <c r="C44" s="1">
-        <v>7.8125E-2</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>410</v>
+        <v>41000</v>
       </c>
       <c r="B45" s="1">
-        <v>1.87692307692307</v>
+        <v>2.6713286713286699</v>
       </c>
       <c r="C45" s="1">
-        <v>6.15384615384615E-2</v>
+        <v>1.3986013986013899E-2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>420</v>
+        <v>42000</v>
       </c>
       <c r="B46" s="1">
-        <v>1.9076923076923</v>
+        <v>2.6643356643356602</v>
       </c>
       <c r="C46" s="1">
-        <v>6.15384615384615E-2</v>
+        <v>2.7972027972027899E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>430</v>
+        <v>43000</v>
       </c>
       <c r="B47" s="1">
-        <v>1.9032258064516101</v>
+        <v>2.5724137931034399</v>
       </c>
       <c r="C47" s="1">
-        <v>6.4516129032257993E-2</v>
+        <v>3.1034482758620599E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>440</v>
+        <v>44000</v>
       </c>
       <c r="B48" s="1">
-        <v>1.96923076923076</v>
+        <v>2.63448275862069</v>
       </c>
       <c r="C48" s="1">
-        <v>4.6153846153846101E-2</v>
+        <v>2.7586206896551699E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>450</v>
+        <v>45000</v>
       </c>
       <c r="B49" s="1">
-        <v>1.9365079365079301</v>
+        <v>2.6275862068965501</v>
       </c>
       <c r="C49" s="1">
-        <v>6.3492063492063405E-2</v>
+        <v>3.1034482758620599E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>460</v>
+        <v>46000</v>
       </c>
       <c r="B50" s="1">
-        <v>1.9365079365079301</v>
+        <v>2.7191780821917799</v>
       </c>
       <c r="C50" s="1">
-        <v>4.7619047619047603E-2</v>
+        <v>1.7123287671232799E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>470</v>
+        <v>47000</v>
       </c>
       <c r="B51" s="1">
-        <v>1.8305084745762701</v>
+        <v>2.66896551724138</v>
       </c>
       <c r="C51" s="1">
-        <v>8.4745762711864403E-2</v>
+        <v>1.72413793103448E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>480</v>
+        <v>48000</v>
       </c>
       <c r="B52" s="1">
-        <v>1.86666666666666</v>
+        <v>2.5782312925170001</v>
       </c>
       <c r="C52" s="1">
-        <v>0.05</v>
+        <v>2.7210884353741398E-2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>490</v>
+        <v>49000</v>
       </c>
       <c r="B53" s="1">
-        <v>1.87096774193548</v>
+        <v>2.6827586206896501</v>
       </c>
       <c r="C53" s="1">
-        <v>4.8387096774193498E-2</v>
+        <v>3.4482758620689599E-2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>500</v>
+        <v>50000</v>
       </c>
       <c r="B54" s="1">
-        <v>1.87692307692307</v>
+        <v>2.6643598615916901</v>
       </c>
       <c r="C54" s="1">
-        <v>6.15384615384615E-2</v>
+        <v>6.9204152249134898E-3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>510</v>
+        <v>51000</v>
       </c>
       <c r="B55" s="1">
-        <v>1.8125</v>
+        <v>2.6484641638225201</v>
       </c>
       <c r="C55" s="1">
-        <v>6.25E-2</v>
+        <v>2.7303754266211601E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>520</v>
+        <v>52000</v>
       </c>
       <c r="B56" s="1">
-        <v>1.9047619047619</v>
+        <v>2.6666666666666599</v>
       </c>
       <c r="C56" s="1">
-        <v>4.7619047619047603E-2</v>
+        <v>2.43055555555555E-2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>530</v>
+        <v>53000</v>
       </c>
       <c r="B57" s="1">
-        <v>1.96969696969696</v>
+        <v>2.7291666666666599</v>
       </c>
       <c r="C57" s="1">
-        <v>4.54545454545454E-2</v>
+        <v>1.7361111111111101E-2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>540</v>
+        <v>54000</v>
       </c>
       <c r="B58" s="1">
-        <v>1.96923076923076</v>
+        <v>2.8373702422145302</v>
       </c>
       <c r="C58" s="1">
-        <v>0.107692307692307</v>
+        <v>1.03806228373702E-2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>550</v>
+        <v>55000</v>
       </c>
       <c r="B59" s="1">
-        <v>1.8412698412698401</v>
+        <v>2.66891891891891</v>
       </c>
       <c r="C59" s="1">
-        <v>9.5238095238095205E-2</v>
+        <v>1.35135135135135E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>560</v>
+        <v>56000</v>
       </c>
       <c r="B60" s="1">
-        <v>1.84848484848484</v>
+        <v>2.6482758620689602</v>
       </c>
       <c r="C60" s="1">
-        <v>6.0606060606060601E-2</v>
+        <v>1.72413793103448E-2</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>570</v>
+        <v>57000</v>
       </c>
       <c r="B61" s="1">
-        <v>2.0579710144927499</v>
+        <v>2.7859649122807002</v>
       </c>
       <c r="C61" s="1">
-        <v>5.7971014492753603E-2</v>
+        <v>1.7543859649122799E-2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>580</v>
+        <v>58000</v>
       </c>
       <c r="B62" s="1">
-        <v>2.0579710144927499</v>
+        <v>2.7298245614034999</v>
       </c>
       <c r="C62" s="1">
-        <v>4.3478260869565202E-2</v>
+        <v>1.7543859649122799E-2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>590</v>
+        <v>59000</v>
       </c>
       <c r="B63" s="1">
-        <v>2.0298507462686501</v>
+        <v>2.63448275862069</v>
       </c>
       <c r="C63" s="1">
-        <v>4.4776119402985003E-2</v>
+        <v>2.0689655172413699E-2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>600</v>
+        <v>60000</v>
       </c>
       <c r="B64" s="1">
-        <v>2.0289855072463698</v>
+        <v>2.8503401360544198</v>
       </c>
       <c r="C64" s="1">
-        <v>5.7971014492753603E-2</v>
+        <v>1.7006802721088399E-2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>610</v>
+        <v>61000</v>
       </c>
       <c r="B65" s="1">
-        <v>1.9393939393939399</v>
+        <v>2.8191126279863399</v>
       </c>
       <c r="C65" s="1">
-        <v>6.0606060606060601E-2</v>
+        <v>1.0238907849829299E-2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>620</v>
+        <v>62000</v>
       </c>
       <c r="B66" s="1">
-        <v>2.0307692307692302</v>
+        <v>2.8333333333333299</v>
       </c>
       <c r="C66" s="1">
-        <v>6.15384615384615E-2</v>
+        <v>2.43055555555555E-2</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>630</v>
+        <v>63000</v>
       </c>
       <c r="B67" s="1">
-        <v>2.0895522388059602</v>
+        <v>2.8356164383561602</v>
       </c>
       <c r="C67" s="1">
-        <v>5.9701492537313397E-2</v>
+        <v>1.7123287671232799E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>640</v>
+        <v>64000</v>
       </c>
       <c r="B68" s="1">
-        <v>1.9375</v>
+        <v>2.7386759581881499</v>
       </c>
       <c r="C68" s="1">
-        <v>3.125E-2</v>
+        <v>1.74216027874564E-2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>650</v>
+        <v>65000</v>
       </c>
       <c r="B69" s="1">
-        <v>1.94029850746268</v>
+        <v>2.8432055749128899</v>
       </c>
       <c r="C69" s="1">
-        <v>1.4925373134328301E-2</v>
+        <v>1.74216027874564E-2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>660</v>
+        <v>66000</v>
       </c>
       <c r="B70" s="1">
-        <v>1.84848484848484</v>
+        <v>2.9652777777777701</v>
       </c>
       <c r="C70" s="1">
-        <v>1.51515151515151E-2</v>
+        <v>1.04166666666666E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>670</v>
+        <v>67000</v>
       </c>
       <c r="B71" s="1">
-        <v>1.8208955223880501</v>
+        <v>2.9379310344827498</v>
       </c>
       <c r="C71" s="1">
-        <v>1.4925373134328301E-2</v>
+        <v>3.4482758620689599E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>680</v>
+        <v>68000</v>
       </c>
       <c r="B72" s="1">
-        <v>1.7878787878787801</v>
+        <v>2.8464163822525599</v>
       </c>
       <c r="C72" s="1">
-        <v>4.54545454545454E-2</v>
+        <v>1.7064846416382201E-2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>690</v>
+        <v>69000</v>
       </c>
       <c r="B73" s="1">
-        <v>1.7538461538461501</v>
+        <v>2.8741258741258702</v>
       </c>
       <c r="C73" s="1">
-        <v>4.6153846153846101E-2</v>
+        <v>1.04895104895104E-2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>700</v>
+        <v>70000</v>
       </c>
       <c r="B74" s="1">
-        <v>1.65625</v>
+        <v>2.8512110726643498</v>
       </c>
       <c r="C74" s="1">
-        <v>6.25E-2</v>
+        <v>2.42214532871972E-2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>710</v>
+        <v>71000</v>
       </c>
       <c r="B75" s="1">
-        <v>1.7538461538461501</v>
+        <v>3.0206896551724101</v>
       </c>
       <c r="C75" s="1">
-        <v>6.15384615384615E-2</v>
+        <v>6.8965517241379301E-3</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>720</v>
+        <v>72000</v>
       </c>
       <c r="B76" s="1">
-        <v>1.6969696969696899</v>
+        <v>2.8996539792387499</v>
       </c>
       <c r="C76" s="1">
-        <v>0.10606060606060599</v>
+        <v>1.03806228373702E-2</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>730</v>
+        <v>73000</v>
       </c>
       <c r="B77" s="1">
-        <v>1.8805970149253699</v>
+        <v>2.8934707903780001</v>
       </c>
       <c r="C77" s="1">
-        <v>2.9850746268656699E-2</v>
+        <v>2.06185567010309E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>740</v>
+        <v>74000</v>
       </c>
       <c r="B78" s="1">
-        <v>1.9090909090909001</v>
+        <v>2.9762711864406701</v>
       </c>
       <c r="C78" s="1">
-        <v>1.51515151515151E-2</v>
+        <v>1.01694915254237E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>750</v>
+        <v>75000</v>
       </c>
       <c r="B79" s="1">
-        <v>1.97058823529411</v>
+        <v>2.86219081272084</v>
       </c>
       <c r="C79" s="1">
-        <v>5.8823529411764698E-2</v>
+        <v>2.8268551236749099E-2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>760</v>
+        <v>76000</v>
       </c>
       <c r="B80" s="1">
-        <v>1.99999999999999</v>
+        <v>2.9484536082474202</v>
       </c>
       <c r="C80" s="1">
-        <v>4.4117647058823498E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>770</v>
+        <v>77000</v>
       </c>
       <c r="B81" s="1">
-        <v>2.0857142857142801</v>
+        <v>2.9140893470790301</v>
       </c>
       <c r="C81" s="1">
-        <v>4.2857142857142802E-2</v>
+        <v>2.06185567010309E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>780</v>
+        <v>78000</v>
       </c>
       <c r="B82" s="1">
-        <v>2.02941176470588</v>
+        <v>2.8827586206896498</v>
       </c>
       <c r="C82" s="1">
-        <v>4.4117647058823498E-2</v>
+        <v>1.3793103448275799E-2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>790</v>
+        <v>79000</v>
       </c>
       <c r="B83" s="1">
-        <v>2</v>
+        <v>3.0779661016949098</v>
       </c>
       <c r="C83" s="1">
-        <v>2.9850746268656699E-2</v>
+        <v>2.0338983050847401E-2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>800</v>
+        <v>80000</v>
       </c>
       <c r="B84" s="1">
-        <v>1.94029850746268</v>
+        <v>2.90592334494773</v>
       </c>
       <c r="C84" s="1">
-        <v>2.9850746268656699E-2</v>
+        <v>1.0452961672473801E-2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>810</v>
+        <v>81000</v>
       </c>
       <c r="B85" s="1">
-        <v>2.0588235294117601</v>
+        <v>2.95138888888888</v>
       </c>
       <c r="C85" s="1">
-        <v>1.47058823529411E-2</v>
+        <v>3.4722222222222199E-3</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>820</v>
+        <v>82000</v>
       </c>
       <c r="B86" s="1">
-        <v>2.0303030303030298</v>
+        <v>2.91525423728813</v>
       </c>
       <c r="C86" s="1">
-        <v>1.51515151515151E-2</v>
+        <v>1.01694915254237E-2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>830</v>
+        <v>83000</v>
       </c>
       <c r="B87" s="1">
-        <v>2</v>
+        <v>2.9895470383275198</v>
       </c>
       <c r="C87" s="1">
-        <v>3.1746031746031703E-2</v>
+        <v>1.39372822299651E-2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>840</v>
+        <v>84000</v>
       </c>
       <c r="B88" s="1">
-        <v>2.12307692307692</v>
+        <v>3.0209790209790199</v>
       </c>
       <c r="C88" s="1">
-        <v>4.6153846153846101E-2</v>
+        <v>3.49650349650349E-3</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>850</v>
+        <v>85000</v>
       </c>
       <c r="B89" s="1">
-        <v>2.09523809523809</v>
+        <v>2.8689655172413802</v>
       </c>
       <c r="C89" s="1">
-        <v>4.7619047619047603E-2</v>
+        <v>6.8965517241379301E-3</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>860</v>
+        <v>86000</v>
       </c>
       <c r="B90" s="1">
-        <v>2.1538461538461502</v>
+        <v>2.8532423208191098</v>
       </c>
       <c r="C90" s="1">
-        <v>6.15384615384615E-2</v>
+        <v>1.36518771331058E-2</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>870</v>
+        <v>87000</v>
       </c>
       <c r="B91" s="1">
-        <v>2.24615384615384</v>
+        <v>2.9010238907849799</v>
       </c>
       <c r="C91" s="1">
-        <v>6.15384615384615E-2</v>
+        <v>6.8259385665529002E-3</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>880</v>
+        <v>88000</v>
       </c>
       <c r="B92" s="1">
-        <v>2.2903225806451601</v>
+        <v>3.1095890410958802</v>
       </c>
       <c r="C92" s="1">
-        <v>3.2258064516128997E-2</v>
+        <v>1.7123287671232799E-2</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>890</v>
+        <v>89000</v>
       </c>
       <c r="B93" s="1">
-        <v>2.2769230769230702</v>
+        <v>3.0726643598615899</v>
       </c>
       <c r="C93" s="1">
-        <v>3.0769230769230702E-2</v>
+        <v>1.73010380622837E-2</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>900</v>
+        <v>90000</v>
       </c>
       <c r="B94" s="1">
-        <v>2.29850746268656</v>
+        <v>2.9863013698630101</v>
       </c>
       <c r="C94" s="1">
-        <v>2.9850746268656699E-2</v>
+        <v>6.8493150684931503E-3</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>910</v>
+        <v>91000</v>
       </c>
       <c r="B95" s="1">
-        <v>2.2089552238805901</v>
+        <v>2.9965397923875399</v>
       </c>
       <c r="C95" s="1">
-        <v>2.9850746268656699E-2</v>
+        <v>1.38408304498269E-2</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>920</v>
+        <v>92000</v>
       </c>
       <c r="B96" s="1">
-        <v>2.1714285714285699</v>
+        <v>3.0174216027874499</v>
       </c>
       <c r="C96" s="1">
-        <v>4.2857142857142802E-2</v>
+        <v>1.39372822299651E-2</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>930</v>
+        <v>93000</v>
       </c>
       <c r="B97" s="1">
-        <v>2.0303030303030298</v>
+        <v>2.8482758620689599</v>
       </c>
       <c r="C97" s="1">
-        <v>6.0606060606060601E-2</v>
+        <v>3.4482758620689598E-3</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>940</v>
+        <v>94000</v>
       </c>
       <c r="B98" s="1">
-        <v>1.9076923076923</v>
+        <v>2.8041237113402002</v>
       </c>
       <c r="C98" s="1">
-        <v>9.2307692307692299E-2</v>
+        <v>6.8728522336769697E-3</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>950</v>
+        <v>95000</v>
       </c>
       <c r="B99" s="1">
-        <v>1.99999999999999</v>
+        <v>2.8384879725085899</v>
       </c>
       <c r="C99" s="1">
-        <v>5.9701492537313397E-2</v>
+        <v>1.37457044673539E-2</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>960</v>
+        <v>96000</v>
       </c>
       <c r="B100" s="1">
-        <v>1.96923076923076</v>
+        <v>2.8767123287671201</v>
       </c>
       <c r="C100" s="1">
-        <v>6.15384615384615E-2</v>
+        <v>1.0273972602739699E-2</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>970</v>
+        <v>97000</v>
       </c>
       <c r="B101" s="1">
-        <v>2.15151515151515</v>
+        <v>2.8591065292096198</v>
       </c>
       <c r="C101" s="1">
-        <v>4.54545454545454E-2</v>
+        <v>1.37457044673539E-2</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>980</v>
+        <v>98000</v>
       </c>
       <c r="B102" s="1">
-        <v>1.99999999999999</v>
+        <v>2.9241379310344802</v>
       </c>
       <c r="C102" s="1">
-        <v>6.15384615384615E-2</v>
+        <v>6.8965517241379301E-3</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>990</v>
+        <v>99000</v>
       </c>
       <c r="B103" s="1">
-        <v>2.14925373134328</v>
+        <v>3.0311418685120999</v>
       </c>
       <c r="C103" s="1">
-        <v>4.4776119402985003E-2</v>
+        <v>1.38408304498269E-2</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>1000</v>
+        <v>100000</v>
       </c>
       <c r="B104" s="1">
-        <v>2.0923076923076902</v>
+        <v>2.9862068965517201</v>
       </c>
       <c r="C104" s="1">
-        <v>3.0769230769230702E-2</v>
+        <v>1.3793103448275799E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit final pour assurer des valeurs koolos
</commit_message>
<xml_diff>
--- a/resultats/simple_execution.xlsx
+++ b/resultats/simple_execution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\5A\OVR_SMA\TP2_tri_collectif_sma\SMA_TP2_Tri_Collectif\resultats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10892657-24DA-4571-9A2A-8E537B53537D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AEC772-B9A1-4EDB-BACC-E187D0F47FC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6B8A2C51-0B39-47A0-BD50-7946639C6253}"/>
   </bookViews>
@@ -122,10 +122,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -207,7 +207,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1128,10 +1128,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1218,7 +1218,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2139,81 +2139,55 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
   <cs:variation>
-    <a:lumMod val="60000"/>
+    <a:tint val="88500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
+    <a:tint val="55000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
+    <a:tint val="75000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
+    <a:tint val="98500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50000"/>
+    <a:tint val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
+    <a:tint val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
+    <a:tint val="80000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
   <cs:variation>
-    <a:lumMod val="60000"/>
+    <a:tint val="88500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
+    <a:tint val="55000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="80000"/>
+    <a:tint val="75000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
+    <a:tint val="98500"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="50000"/>
+    <a:tint val="30000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
+    <a:tint val="60000"/>
   </cs:variation>
   <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
+    <a:tint val="80000"/>
   </cs:variation>
 </cs:colorStyle>
 </file>
@@ -3631,7 +3605,7 @@
   <dimension ref="A1:H104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>